<commit_message>
Display tree from Excel
</commit_message>
<xml_diff>
--- a/CatTree.xlsx
+++ b/CatTree.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcyuser/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcyuser/Desktop/CatTree-Lite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5355976C-47EB-4A46-AFA6-3810AD686439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208A26FD-A6AB-1B4F-989F-065DA1C24A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="2760" windowWidth="22420" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3740" yWindow="1320" windowWidth="22420" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="0" sheetId="2" r:id="rId1"/>
+    <sheet name="第一棵分類樹" sheetId="2" r:id="rId1"/>
+    <sheet name="第二棵分類樹" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="valHighlight">#REF!</definedName>
@@ -31,25 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>序號</t>
-  </si>
-  <si>
-    <t>文本內容</t>
-  </si>
-  <si>
-    <t>自訂欄位一</t>
-  </si>
-  <si>
-    <t>自訂欄位二</t>
-  </si>
-  <si>
-    <t>使用者可自行新增欄位及設定欄位名稱。以「時間」為例。</t>
-  </si>
-  <si>
-    <t>使用者可自行新增欄位及設定欄位名稱。以「地點」為例。</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>id</t>
   </si>
@@ -57,74 +40,424 @@
     <t>text</t>
   </si>
   <si>
-    <t>時間</t>
-  </si>
-  <si>
-    <t>地點</t>
-  </si>
-  <si>
-    <t>國立臺灣大學</t>
-  </si>
-  <si>
-    <t>民國108年</t>
-  </si>
-  <si>
-    <t>臺灣–臺北</t>
-  </si>
-  <si>
-    <t>為系統指定欄位名稱。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>分類</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>text 欄位可輸入文本內容，在 CatTree Lite 便於瀏覽文本內容。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CatTree_我的分類</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>鴻厖氏紀/涇陽王/–/–;鴻厖氏紀/貉龍君/–/–</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>為系統指定欄位名稱。放入分類結果，可以多值，並以逗號分隔。CatTree_我的分類為樹的名稱，在此樹根就會叫做我的分類。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CatTree_我的分類2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>為系統指定欄位名稱。放入分類結果，可以多值，並以逗號分隔。CatTree_我的分類2為樹的名稱，在此樹根就會叫做我的分類2。</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>宗教/廟宇/1;宗教/廟宇/故事</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>L1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>地點</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立臺灣大學</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>108</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺北</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立清華大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>新竹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立交通大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立政治大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺北</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>民事</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>田房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>霸佔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爭界</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>國立臺灣大學1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立清華大學</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立交通大學</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立政治大學</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>族群關係</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客家內部關係</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金錢糾紛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>社會組織</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拓墾組織</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.google.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -140,16 +473,15 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="9"/>
+      <name val="Noto Sans CJK TC Black"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -174,12 +506,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -493,103 +824,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E926FAD3-25CD-5941-B3E2-B7F949393868}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" customWidth="1"/>
-    <col min="2" max="3" width="42.3984375" customWidth="1"/>
-    <col min="4" max="4" width="27.59765625" customWidth="1"/>
-    <col min="5" max="5" width="20.19921875" customWidth="1"/>
-    <col min="6" max="6" width="34.19921875" customWidth="1"/>
+    <col min="1" max="5" width="19.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.19921875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="34.19921875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.3984375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="H5" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE67B9AC-C9F4-E245-A33A-5F8583CF95D6}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.796875" customWidth="1"/>
+    <col min="3" max="3" width="32.59765625" customWidth="1"/>
+    <col min="4" max="4" width="25.19921875" customWidth="1"/>
+    <col min="5" max="5" width="47.796875" customWidth="1"/>
+    <col min="6" max="6" width="40.796875" customWidth="1"/>
+    <col min="7" max="7" width="24.3984375" customWidth="1"/>
+    <col min="8" max="8" width="41.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1">
+        <v>123</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Display tree from Excel and add error proof on tree level of Excel
</commit_message>
<xml_diff>
--- a/CatTree.xlsx
+++ b/CatTree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcyuser/Desktop/CatTree-Lite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208A26FD-A6AB-1B4F-989F-065DA1C24A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7B7B68-A8B8-0D47-91A4-7D8B2436B242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="1320" windowWidth="22420" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2260" yWindow="1580" windowWidth="26460" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="第一棵分類樹" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -89,17 +91,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>國立臺灣大學</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>民國</t>
     </r>
     <r>
@@ -158,18 +149,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>國立清華大學</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>民國</t>
     </r>
     <r>
@@ -230,18 +209,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>國立交通大學</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t>民國</t>
     </r>
     <r>
@@ -261,18 +228,6 @@
         <family val="2"/>
       </rPr>
       <t>年</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>國立政治大學</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -440,18 +395,316 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://www.google.com</t>
+  </si>
+  <si>
+    <t>1_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3_text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_時間</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4_地點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5_Url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6_RefId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>twgis_19291</t>
+  </si>
+  <si>
+    <t>hvd_70623</t>
+  </si>
+  <si>
+    <t>cbdb_196395</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dila_A000294</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立臺灣大學</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>108</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺北</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立清華大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>新竹</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立交通大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>110</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>國立政治大學</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>民國</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>111</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺灣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>–</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>臺北</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://140.112.114.10/</t>
+  </si>
+  <si>
+    <t>IiifManifest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://iiif.lib.harvard.edu/manifests/ids:3098346</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -485,6 +738,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -506,11 +778,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -824,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E926FAD3-25CD-5941-B3E2-B7F949393868}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -837,139 +1113,158 @@
     <col min="7" max="7" width="20.19921875" style="2" customWidth="1"/>
     <col min="8" max="8" width="34.19921875" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.3984375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="11" style="2"/>
+    <col min="10" max="10" width="19" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>33</v>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="1" t="s">
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4">
         <v>123</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
+      <c r="F5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -980,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE67B9AC-C9F4-E245-A33A-5F8583CF95D6}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -995,9 +1290,10 @@
     <col min="6" max="6" width="40.796875" customWidth="1"/>
     <col min="7" max="7" width="24.3984375" customWidth="1"/>
     <col min="8" max="8" width="41.19921875" customWidth="1"/>
+    <col min="9" max="9" width="19" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,125 +1318,134 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I1" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
+      <c r="I2" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1">
         <v>123</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
postMessage with ExcelMessage as input
</commit_message>
<xml_diff>
--- a/CatTree.xlsx
+++ b/CatTree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcyuser/Desktop/CatTree-Lite/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7B7B68-A8B8-0D47-91A4-7D8B2436B242}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13EE0E5B-9E80-0846-91D3-C6CE0456237F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2260" yWindow="1580" windowWidth="26460" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -414,14 +414,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5_Url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6_RefId</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>twgis_19291</t>
   </si>
   <si>
@@ -698,6 +690,18 @@
   </si>
   <si>
     <t>https://iiif.lib.harvard.edu/manifests/ids:3098346</t>
+  </si>
+  <si>
+    <t>5_RefId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6_Url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爭界123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1103,7 +1107,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1143,10 +1147,10 @@
         <v>33</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1164,19 +1168,19 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>29</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1194,19 +1198,19 @@
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="I3" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1220,23 +1224,23 @@
         <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1254,17 +1258,17 @@
         <v>123</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
@@ -1346,7 +1350,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">

</xml_diff>